<commit_message>
fixed error i results-sizes plot
</commit_message>
<xml_diff>
--- a/results/results-sizes-small.xlsx
+++ b/results/results-sizes-small.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils\Documents\Studium\TUM\09_Masterarbeit\master-thesis-tests\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF268E2-6379-4285-9D21-7410A473AA99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6F8FB-7816-4155-9E57-B1C736EFEAA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10A37585-0CE9-42C1-8EEA-BBFDD8762655}"/>
   </bookViews>
@@ -33,12 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
-    <t>m = 20</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>α</t>
   </si>
   <si>
@@ -61,6 +55,12 @@
   </si>
   <si>
     <t>star tree - setup 2</t>
+  </si>
+  <si>
+    <t>k = 20</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,23 +700,23 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="31"/>
       <c r="F1" s="37"/>
       <c r="G1" s="30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
       <c r="J1" s="37"/>
       <c r="K1" s="30" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L1" s="31"/>
       <c r="M1" s="31"/>
@@ -725,46 +725,46 @@
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="G2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="J2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="L2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="N2" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O2" s="15"/>
     </row>

</xml_diff>

<commit_message>
added comparison for tests
</commit_message>
<xml_diff>
--- a/results/results-sizes-small.xlsx
+++ b/results/results-sizes-small.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils\Documents\Studium\TUM\09_Masterarbeit\master-thesis-tests\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6F8FB-7816-4155-9E57-B1C736EFEAA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46C79AD-71BB-4921-96FE-09BE95D6ED56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10A37585-0CE9-42C1-8EEA-BBFDD8762655}"/>
   </bookViews>
@@ -109,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -251,11 +251,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,6 +413,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -381,6 +457,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>35472</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>216118</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Textfeld 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A5A450D-E930-44D2-8F03-97416B369B19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5645369" y="2022584"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -680,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DE9B96-2516-48F5-9B22-0E368715A17B}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +834,7 @@
     <col min="14" max="14" width="6.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>8</v>
       </c>
@@ -723,7 +859,7 @@
       <c r="N1" s="31"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -767,8 +903,10 @@
         <v>1</v>
       </c>
       <c r="O2" s="15"/>
-    </row>
-    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+    </row>
+    <row r="3" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32">
         <v>100</v>
       </c>
@@ -813,7 +951,7 @@
       </c>
       <c r="O3" s="15"/>
     </row>
-    <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
       <c r="B4" s="2">
         <v>0.05</v>
@@ -856,7 +994,7 @@
       </c>
       <c r="O4" s="15"/>
     </row>
-    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="3">
         <v>0.1</v>
@@ -899,7 +1037,7 @@
       </c>
       <c r="O5" s="15"/>
     </row>
-    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32">
         <v>250</v>
       </c>
@@ -943,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32"/>
       <c r="B7" s="2">
         <v>0.05</v>
@@ -986,7 +1124,7 @@
       </c>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="3">
         <v>0.1</v>
@@ -1029,7 +1167,7 @@
       </c>
       <c r="O8" s="15"/>
     </row>
-    <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32">
         <v>500</v>
       </c>
@@ -1074,7 +1212,7 @@
       </c>
       <c r="O9" s="15"/>
     </row>
-    <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32"/>
       <c r="B10" s="2">
         <v>0.05</v>
@@ -1117,7 +1255,7 @@
       </c>
       <c r="O10" s="15"/>
     </row>
-    <row r="11" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32"/>
       <c r="B11" s="3">
         <v>0.1</v>
@@ -1134,33 +1272,33 @@
       <c r="F11" s="11">
         <v>0.10199999999999999</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="19">
         <v>0.08</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="14">
         <v>0.124</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="14">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="25">
         <v>0.74</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="9">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="14">
         <v>0.11600000000000001</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="14">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="22">
         <v>0.08</v>
       </c>
       <c r="O11" s="15"/>
     </row>
-    <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
         <v>1000</v>
       </c>
@@ -1179,33 +1317,33 @@
       <c r="F12" s="14">
         <v>1.2E-2</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="42">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="41">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="41">
         <v>1.2E-2</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="40">
         <v>0.85599999999999998</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="42">
         <v>2E-3</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="41">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="45">
         <v>0</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="41">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="O12" s="15"/>
     </row>
-    <row r="13" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
       <c r="B13" s="27">
         <v>0.05</v>
@@ -1222,7 +1360,7 @@
       <c r="F13" s="14">
         <v>6.2E-2</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="43">
         <v>0.03</v>
       </c>
       <c r="H13" s="22">
@@ -1231,10 +1369,10 @@
       <c r="I13" s="14">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="14">
         <v>0.94399999999999995</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="38">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="L13" s="22">
@@ -1248,7 +1386,7 @@
       </c>
       <c r="O13" s="15"/>
     </row>
-    <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
       <c r="B14" s="27">
         <v>0.1</v>
@@ -1262,10 +1400,10 @@
       <c r="E14" s="14">
         <v>6.2E-2</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="44">
         <v>0.11</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="14">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="H14" s="14">
@@ -1274,7 +1412,7 @@
       <c r="I14" s="22">
         <v>0.11</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="39">
         <v>0.96199999999999997</v>
       </c>
       <c r="K14" s="14">
@@ -1291,7 +1429,7 @@
       </c>
       <c r="O14" s="15"/>
     </row>
-    <row r="15" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1302,7 +1440,7 @@
       <c r="N15" s="7"/>
       <c r="O15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1354,5 +1492,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>